<commit_message>
Add tests for ReadTableFromExcel for numeric column headings and to better handle include and exclude filters.
</commit_message>
<xml_diff>
--- a/test/regression/commands/general/ReadTableFromExcel/Data/TestWorkbook.xlsx
+++ b/test/regression/commands/general/ReadTableFromExcel/Data/TestWorkbook.xlsx
@@ -1,18 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\owf-gitrepos\cdss-app-tstool-test\test\regression\commands\general\ReadTableFromExcel\Data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="18075" windowHeight="8445" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="18072" windowHeight="8448" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Address_NoFormulas" sheetId="1" r:id="rId1"/>
-    <sheet name="Address_Formulas" sheetId="4" r:id="rId2"/>
-    <sheet name="Worksheet_NoHeaders" sheetId="3" r:id="rId3"/>
-    <sheet name="Worksheet_Headers" sheetId="2" r:id="rId4"/>
+    <sheet name="ExcludeMultiple" sheetId="6" r:id="rId2"/>
+    <sheet name="Address_Formulas" sheetId="4" r:id="rId3"/>
+    <sheet name="NumericHeadings" sheetId="5" r:id="rId4"/>
+    <sheet name="Worksheet_NoHeaders" sheetId="3" r:id="rId5"/>
+    <sheet name="Worksheet_Headers" sheetId="2" r:id="rId6"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -22,7 +29,7 @@
     <author>Steve Malers</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -35,7 +42,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -48,7 +55,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -61,7 +68,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -74,7 +81,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -97,7 +104,7 @@
     <author>Steve Malers</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -110,7 +117,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -123,7 +130,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -136,7 +143,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -149,7 +156,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -172,7 +179,7 @@
     <author>Steve Malers</author>
   </authors>
   <commentList>
-    <comment ref="A1" authorId="0">
+    <comment ref="A1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -185,7 +192,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B1" authorId="0">
+    <comment ref="B1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +205,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C1" authorId="0">
+    <comment ref="C1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -211,7 +218,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E1" authorId="0">
+    <comment ref="E1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -224,7 +231,157 @@
         </r>
       </text>
     </comment>
-    <comment ref="F1" authorId="0">
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column formatted as date/time.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments4.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Steve Malers</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column has no formatting.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column is formatted as number with decimals=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column is formatted as number with decimals=2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column formatted as date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column formatted as date/time.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments5.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Steve Malers</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column has no formatting.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column is formatted as number with decimals=0</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column is formatted as number with decimals=2</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="8"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Column formatted as date</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -242,7 +399,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="18">
   <si>
     <t>String 1</t>
   </si>
@@ -291,15 +448,21 @@
   <si>
     <t>Column7_Boolean</t>
   </si>
+  <si>
+    <t>aString 6</t>
+  </si>
+  <si>
+    <t>bString 10</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="m/d/yy\ h:mm;@"/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -346,6 +509,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -392,7 +563,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -424,9 +595,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -458,6 +630,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -633,25 +806,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A9" sqref="A9:XFD9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="21.140625" customWidth="1"/>
-    <col min="2" max="2" width="16.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -674,7 +847,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
@@ -697,7 +870,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -714,7 +887,7 @@
         <v>40910.083333333336</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
@@ -737,7 +910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>
@@ -758,7 +931,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104</v>
       </c>
@@ -781,7 +954,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>105</v>
       </c>
@@ -802,7 +975,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>106</v>
       </c>
@@ -825,7 +998,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>107</v>
       </c>
@@ -843,7 +1016,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>108</v>
       </c>
@@ -861,7 +1034,7 @@
         <v>40917.375</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>109</v>
       </c>
@@ -892,25 +1065,283 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+      <c r="D1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F1" t="s">
+        <v>14</v>
+      </c>
+      <c r="G1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40909</v>
+      </c>
+      <c r="F2" s="4">
+        <v>40909.041666666664</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.02</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40910</v>
+      </c>
+      <c r="F3" s="4">
+        <v>40910.083333333336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40911</v>
+      </c>
+      <c r="F4" s="4">
+        <v>40911.125</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3">
+        <v>4.04</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40912</v>
+      </c>
+      <c r="F5" s="4">
+        <v>40912.166666666664</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.05</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40913</v>
+      </c>
+      <c r="F6" s="4">
+        <v>40913.208333333336</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="1">
+        <v>40914</v>
+      </c>
+      <c r="F7" s="4">
+        <v>40914.25</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7.07</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>40915</v>
+      </c>
+      <c r="F8" s="4">
+        <v>40915.291666666664</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8.08</v>
+      </c>
+      <c r="E9" s="1">
+        <v>40916</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9.09</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4">
+        <v>40917.375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E11" s="1">
+        <v>40918</v>
+      </c>
+      <c r="F11" s="4">
+        <v>40918.416666666664</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <legacyDrawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
       <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" customWidth="1"/>
-    <col min="2" max="2" width="18.140625" customWidth="1"/>
-    <col min="3" max="3" width="18.85546875" customWidth="1"/>
-    <col min="4" max="4" width="16.28515625" customWidth="1"/>
-    <col min="5" max="5" width="15.28515625" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.42578125" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" customWidth="1"/>
+    <col min="2" max="2" width="18.109375" customWidth="1"/>
+    <col min="3" max="3" width="18.88671875" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="15.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="19.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>"Column"&amp;TEXT(COLUMN(),"0")&amp;"_General"</f>
         <v>Column1_General</v>
@@ -940,7 +1371,7 @@
         <v>Column7_Boolean</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <f>100 + (ROW() - 2)</f>
         <v>100</v>
@@ -968,7 +1399,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <f t="shared" ref="B3:B11" si="0">ROW()-1</f>
         <v>2</v>
@@ -988,7 +1419,7 @@
         <v>40910.083333333336</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>100 + (ROW() - 2)</f>
         <v>102</v>
@@ -1016,7 +1447,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" ref="A5:A11" si="3">100 + (ROW() - 2)</f>
         <v>103</v>
@@ -1041,7 +1472,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="3"/>
         <v>104</v>
@@ -1069,7 +1500,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="3"/>
         <v>105</v>
@@ -1094,7 +1525,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="3"/>
         <v>106</v>
@@ -1122,7 +1553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="3"/>
         <v>107</v>
@@ -1144,7 +1575,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="3"/>
         <v>108</v>
@@ -1166,7 +1597,7 @@
         <v>40917.375</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="3"/>
         <v>109</v>
@@ -1201,26 +1632,285 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.109375" customWidth="1"/>
+    <col min="2" max="2" width="16.44140625" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="16.33203125" customWidth="1"/>
+    <col min="5" max="5" width="17.44140625" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="20.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1">
+        <v>1990</v>
+      </c>
+      <c r="C1">
+        <v>1991</v>
+      </c>
+      <c r="D1">
+        <v>1992</v>
+      </c>
+      <c r="E1" s="2">
+        <v>1993.3</v>
+      </c>
+      <c r="F1" s="2">
+        <v>1994</v>
+      </c>
+      <c r="G1">
+        <v>1995</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>100</v>
+      </c>
+      <c r="B2" s="2">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3">
+        <v>1.01</v>
+      </c>
+      <c r="D2" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="1">
+        <v>40909</v>
+      </c>
+      <c r="F2" s="4">
+        <v>40909.041666666664</v>
+      </c>
+      <c r="G2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B3" s="2">
+        <v>2</v>
+      </c>
+      <c r="C3" s="3">
+        <v>2.02</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="1">
+        <v>40910</v>
+      </c>
+      <c r="F3" s="4">
+        <v>40910.083333333336</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>102</v>
+      </c>
+      <c r="B4" s="2">
+        <v>3</v>
+      </c>
+      <c r="C4" s="3">
+        <v>3.03</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="1">
+        <v>40911</v>
+      </c>
+      <c r="F4" s="4">
+        <v>40911.125</v>
+      </c>
+      <c r="G4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>103</v>
+      </c>
+      <c r="B5" s="2"/>
+      <c r="C5" s="3">
+        <v>4.04</v>
+      </c>
+      <c r="D5" t="s">
+        <v>3</v>
+      </c>
+      <c r="E5" s="1">
+        <v>40912</v>
+      </c>
+      <c r="F5" s="4">
+        <v>40912.166666666664</v>
+      </c>
+      <c r="G5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>104</v>
+      </c>
+      <c r="B6" s="2">
+        <v>5</v>
+      </c>
+      <c r="C6" s="3">
+        <v>5.05</v>
+      </c>
+      <c r="D6" t="s">
+        <v>4</v>
+      </c>
+      <c r="E6" s="1">
+        <v>40913</v>
+      </c>
+      <c r="F6" s="4">
+        <v>40913.208333333336</v>
+      </c>
+      <c r="G6" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>105</v>
+      </c>
+      <c r="B7" s="2">
+        <v>6</v>
+      </c>
+      <c r="C7" s="3"/>
+      <c r="D7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="1">
+        <v>40914</v>
+      </c>
+      <c r="F7" s="4">
+        <v>40914.25</v>
+      </c>
+      <c r="G7" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>106</v>
+      </c>
+      <c r="B8" s="2">
+        <v>7</v>
+      </c>
+      <c r="C8" s="3">
+        <v>7.07</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" s="1">
+        <v>40915</v>
+      </c>
+      <c r="F8" s="4">
+        <v>40915.291666666664</v>
+      </c>
+      <c r="G8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>107</v>
+      </c>
+      <c r="B9" s="2">
+        <v>8</v>
+      </c>
+      <c r="C9" s="3">
+        <v>8.08</v>
+      </c>
+      <c r="E9" s="1">
+        <v>40916</v>
+      </c>
+      <c r="F9" s="4"/>
+      <c r="G9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>108</v>
+      </c>
+      <c r="B10" s="2">
+        <v>9</v>
+      </c>
+      <c r="C10" s="3">
+        <v>9.09</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="4">
+        <v>40917.375</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>109</v>
+      </c>
+      <c r="B11" s="2">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <v>10.1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>8</v>
+      </c>
+      <c r="E11" s="1">
+        <v>40918</v>
+      </c>
+      <c r="F11" s="4">
+        <v>40918.416666666664</v>
+      </c>
+      <c r="G11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.5703125" customWidth="1"/>
-    <col min="2" max="2" width="18.7109375" customWidth="1"/>
+    <col min="1" max="1" width="20.5546875" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" customWidth="1"/>
     <col min="3" max="3" width="19" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" customWidth="1"/>
+    <col min="4" max="4" width="16.44140625" customWidth="1"/>
     <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="15.85546875" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>100</v>
       </c>
@@ -1243,7 +1933,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B2" s="2">
         <v>2</v>
       </c>
@@ -1260,7 +1950,7 @@
         <v>40910.083333333336</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>102</v>
       </c>
@@ -1283,7 +1973,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>103</v>
       </c>
@@ -1304,7 +1994,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>104</v>
       </c>
@@ -1327,7 +2017,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>105</v>
       </c>
@@ -1348,7 +2038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>106</v>
       </c>
@@ -1371,7 +2061,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>107</v>
       </c>
@@ -1389,7 +2079,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>108</v>
       </c>
@@ -1407,7 +2097,7 @@
         <v>40917.375</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>109</v>
       </c>
@@ -1435,26 +2125,26 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.7109375" customWidth="1"/>
-    <col min="2" max="2" width="20.5703125" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.42578125" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.85546875" customWidth="1"/>
-    <col min="7" max="7" width="22.28515625" customWidth="1"/>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.5546875" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
+    <col min="4" max="4" width="17.44140625" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
+    <col min="6" max="6" width="18.88671875" customWidth="1"/>
+    <col min="7" max="7" width="22.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1477,7 +2167,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>100</v>
       </c>
@@ -1500,7 +2190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="B3" s="2">
         <v>2</v>
       </c>
@@ -1517,7 +2207,7 @@
         <v>40910.083333333336</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>102</v>
       </c>
@@ -1540,7 +2230,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>103</v>
       </c>
@@ -1561,7 +2251,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>104</v>
       </c>
@@ -1584,7 +2274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>105</v>
       </c>
@@ -1605,7 +2295,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>106</v>
       </c>
@@ -1628,7 +2318,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>107</v>
       </c>
@@ -1646,7 +2336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>108</v>
       </c>
@@ -1664,7 +2354,7 @@
         <v>40917.375</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>109</v>
       </c>

</xml_diff>